<commit_message>
Excel with data tables.
</commit_message>
<xml_diff>
--- a/Docs/Attachments/BenchmarksVitis.xlsx
+++ b/Docs/Attachments/BenchmarksVitis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\c-sharp\Hastlayer-SDK-Vitis\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\c-sharp\Hastlayer-SDK-Vitis\Docs\Attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DDF9C8-FFC6-4BC1-B71D-539E3087D0E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14311D84-2C93-4D69-A776-DDE853578861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,8 +103,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0\ &quot;ms&quot;"/>
     <numFmt numFmtId="165" formatCode="0\ &quot;Ws&quot;"/>
-    <numFmt numFmtId="171" formatCode="0.00\ &quot;W&quot;"/>
-    <numFmt numFmtId="172" formatCode="0.00\ &quot;Ws&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.00\ &quot;W&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00\ &quot;Ws&quot;"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -589,8 +589,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -636,7 +636,35 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;W&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00\ &quot;Ws&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0\ &quot;ms&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0\ &quot;ms&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0\ &quot;Ws&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0\ &quot;ms&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -647,6 +675,38 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DEFFE78-E3D4-4B7C-9C40-A543930B7FFC}" name="Table1" displayName="Table1" ref="A1:L17" totalsRowShown="0">
+  <autoFilter ref="A1:L17" xr:uid="{8A2D4EA8-9217-4FE5-8D42-089013CF93D2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
+    <sortCondition ref="A1:A17"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{BCC5BB97-9D21-4C10-A1AC-3169285ACE85}" name="Device"/>
+    <tableColumn id="2" xr3:uid="{E02FF3CC-EF4B-449F-AC35-450BFA13E16F}" name="Algorithm"/>
+    <tableColumn id="3" xr3:uid="{B6499BAC-6A77-45CF-B33A-7834EF7AE07C}" name="Speed advantage" dataDxfId="8">
+      <calculatedColumnFormula>(F2/J2)-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F534939D-7296-49EA-94FA-117E5B1AD75B}" name="Power advantage" dataDxfId="7">
+      <calculatedColumnFormula>(G2/K2)-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{9821B29C-FCB1-4C03-A563-1B6291E9CD28}" name="Parallelism"/>
+    <tableColumn id="6" xr3:uid="{D59DCF9C-205F-4833-9388-5263C54DDB8B}" name="CPU" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{1A2039BF-94BA-4B94-903A-588CED48280E}" name="CPU power" dataDxfId="5">
+      <calculatedColumnFormula>90*F2/1000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{9D77DFD2-A1F6-455B-A5A6-964B37E62FC4}" name="FPGA utilization" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{0F2C4863-589C-42AC-8BB0-D5F5238E5C6A}" name="Net FPGA" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{17AEC27A-0BAE-4DDB-9FB3-19107E161C70}" name="Total FPGA" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{55E77FEE-ED30-4B73-AE7C-435553A4B7D0}" name="FPGA power" dataDxfId="1">
+      <calculatedColumnFormula>L2*J2/1000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{FA68E0D5-D0B6-4FBF-9069-693603D766A2}" name="FPGA on-chip power" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -949,23 +1009,23 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="4" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1056,11 +1116,11 @@
         <v>14</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C17" si="0">(F3/J3)-1</f>
+        <f>(F3/J3)-1</f>
         <v>34.4765485141425</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D17" si="1">(G3/K3)-1</f>
+        <f>(G3/K3)-1</f>
         <v>132.65521228485181</v>
       </c>
       <c r="E3">
@@ -1070,7 +1130,7 @@
         <v>198172</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" ref="G3:G17" si="2">90*F3/1000</f>
+        <f>90*F3/1000</f>
         <v>17835.48</v>
       </c>
       <c r="H3" s="1">
@@ -1083,7 +1143,7 @@
         <v>5586</v>
       </c>
       <c r="K3" s="6">
-        <f t="shared" ref="K3:K17" si="3">L3*J3/1000</f>
+        <f>L3*J3/1000</f>
         <v>133.44395399999999</v>
       </c>
       <c r="L3" s="5">
@@ -1098,11 +1158,11 @@
         <v>15</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" si="0"/>
+        <f>(F4/J4)-1</f>
         <v>1.7071428571428573</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="1"/>
+        <f>(G4/K4)-1</f>
         <v>14.642196786264583</v>
       </c>
       <c r="E4">
@@ -1112,7 +1172,7 @@
         <v>379</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F4/1000</f>
         <v>34.11</v>
       </c>
       <c r="H4" s="1">
@@ -1125,7 +1185,7 @@
         <v>140</v>
       </c>
       <c r="K4" s="6">
-        <f t="shared" si="3"/>
+        <f>L4*J4/1000</f>
         <v>2.1806399999999999</v>
       </c>
       <c r="L4" s="5">
@@ -1140,11 +1200,11 @@
         <v>16</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="0"/>
+        <f>(F5/J5)-1</f>
         <v>2.0298507462686568</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="1"/>
+        <f>(G5/K5)-1</f>
         <v>13.325535443350622</v>
       </c>
       <c r="E5">
@@ -1154,7 +1214,7 @@
         <v>203</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F5/1000</f>
         <v>18.27</v>
       </c>
       <c r="H5" s="1">
@@ -1167,7 +1227,7 @@
         <v>67</v>
       </c>
       <c r="K5" s="6">
-        <f t="shared" si="3"/>
+        <f>L5*J5/1000</f>
         <v>1.275345</v>
       </c>
       <c r="L5" s="5">
@@ -1182,11 +1242,11 @@
         <v>13</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
+        <f>(F6/J6)-1</f>
         <v>15.030303030303031</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="1"/>
+        <f>(G6/K6)-1</f>
         <v>56.214755422242725</v>
       </c>
       <c r="E6">
@@ -1196,7 +1256,7 @@
         <v>529</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F6/1000</f>
         <v>47.61</v>
       </c>
       <c r="H6" s="1">
@@ -1209,7 +1269,7 @@
         <v>33</v>
       </c>
       <c r="K6" s="6">
-        <f t="shared" si="3"/>
+        <f>L6*J6/1000</f>
         <v>0.83212800000000009</v>
       </c>
       <c r="L6" s="5">
@@ -1224,11 +1284,11 @@
         <v>14</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="0"/>
+        <f>(F7/J7)-1</f>
         <v>32.680557977332171</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="1"/>
+        <f>(G7/K7)-1</f>
         <v>119.21138237467859</v>
       </c>
       <c r="E7">
@@ -1238,7 +1298,7 @@
         <v>193158</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F7/1000</f>
         <v>17384.22</v>
       </c>
       <c r="H7" s="1">
@@ -1251,7 +1311,7 @@
         <v>5735</v>
       </c>
       <c r="K7" s="6">
-        <f t="shared" si="3"/>
+        <f>L7*J7/1000</f>
         <v>144.61376000000001</v>
       </c>
       <c r="L7" s="5">
@@ -1266,11 +1326,11 @@
         <v>15</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="0"/>
+        <f>(F8/J8)-1</f>
         <v>3.568807339449541</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="1"/>
+        <f>(G8/K8)-1</f>
         <v>24.371300089495815</v>
       </c>
       <c r="E8">
@@ -1280,7 +1340,7 @@
         <v>498</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F8/1000</f>
         <v>44.82</v>
       </c>
       <c r="H8" s="1">
@@ -1293,7 +1353,7 @@
         <v>109</v>
       </c>
       <c r="K8" s="6">
-        <f t="shared" si="3"/>
+        <f>L8*J8/1000</f>
         <v>1.7665630000000001</v>
       </c>
       <c r="L8" s="5">
@@ -1308,11 +1368,11 @@
         <v>16</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="0"/>
+        <f>(F9/J9)-1</f>
         <v>3.6904761904761907</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="1"/>
+        <f>(G9/K9)-1</f>
         <v>20.222807156143844</v>
       </c>
       <c r="E9">
@@ -1322,7 +1382,7 @@
         <v>197</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F9/1000</f>
         <v>17.73</v>
       </c>
       <c r="H9" s="1">
@@ -1335,7 +1395,7 @@
         <v>42</v>
       </c>
       <c r="K9" s="6">
-        <f t="shared" si="3"/>
+        <f>L9*J9/1000</f>
         <v>0.83542199999999989</v>
       </c>
       <c r="L9" s="5">
@@ -1350,11 +1410,11 @@
         <v>13</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="0"/>
+        <f>(F10/J10)-1</f>
         <v>15.90625</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="1"/>
+        <f>(G10/K10)-1</f>
         <v>65.054373779031906</v>
       </c>
       <c r="E10">
@@ -1364,7 +1424,7 @@
         <v>541</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F10/1000</f>
         <v>48.69</v>
       </c>
       <c r="H10" s="1">
@@ -1377,7 +1437,7 @@
         <v>32</v>
       </c>
       <c r="K10" s="6">
-        <f t="shared" si="3"/>
+        <f>L10*J10/1000</f>
         <v>0.73712</v>
       </c>
       <c r="L10" s="5">
@@ -1392,11 +1452,11 @@
         <v>19</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="0"/>
+        <f>(F11/J11)-1</f>
         <v>34.139676113360323</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="1"/>
+        <f>(G11/K11)-1</f>
         <v>136.29415455621572</v>
       </c>
       <c r="E11">
@@ -1406,7 +1466,7 @@
         <v>17359</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F11/1000</f>
         <v>1562.31</v>
       </c>
       <c r="H11" s="1">
@@ -1419,7 +1479,7 @@
         <v>494</v>
       </c>
       <c r="K11" s="6">
-        <f t="shared" si="3"/>
+        <f>L11*J11/1000</f>
         <v>11.379290000000001</v>
       </c>
       <c r="L11" s="5">
@@ -1434,11 +1494,11 @@
         <v>15</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="0"/>
+        <f>(F12/J12)-1</f>
         <v>2.2612612612612613</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="1"/>
+        <f>(G12/K12)-1</f>
         <v>18.583234154891482</v>
       </c>
       <c r="E12">
@@ -1448,7 +1508,7 @@
         <v>362</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F12/1000</f>
         <v>32.58</v>
       </c>
       <c r="H12" s="1">
@@ -1461,7 +1521,7 @@
         <v>111</v>
       </c>
       <c r="K12" s="6">
-        <f t="shared" si="3"/>
+        <f>L12*J12/1000</f>
         <v>1.6636679999999999</v>
       </c>
       <c r="L12" s="5">
@@ -1476,11 +1536,11 @@
         <v>16</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="0"/>
+        <f>(F13/J13)-1</f>
         <v>3.8684210526315788</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="1"/>
+        <f>(G13/K13)-1</f>
         <v>23.966261808367072</v>
       </c>
       <c r="E13">
@@ -1490,7 +1550,7 @@
         <v>185</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F13/1000</f>
         <v>16.649999999999999</v>
       </c>
       <c r="H13" s="1">
@@ -1503,7 +1563,7 @@
         <v>38</v>
       </c>
       <c r="K13" s="6">
-        <f t="shared" si="3"/>
+        <f>L13*J13/1000</f>
         <v>0.66689999999999994</v>
       </c>
       <c r="L13" s="5">
@@ -1518,11 +1578,11 @@
         <v>13</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="0"/>
+        <f>(F14/J14)-1</f>
         <v>13.242424242424242</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="1"/>
+        <f>(G14/K14)-1</f>
         <v>63.588238527571392</v>
       </c>
       <c r="E14">
@@ -1532,7 +1592,7 @@
         <v>470</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F14/1000</f>
         <v>42.3</v>
       </c>
       <c r="H14" s="1">
@@ -1545,7 +1605,7 @@
         <v>33</v>
       </c>
       <c r="K14" s="6">
-        <f t="shared" si="3"/>
+        <f>L14*J14/1000</f>
         <v>0.654918</v>
       </c>
       <c r="L14" s="5">
@@ -1560,11 +1620,11 @@
         <v>19</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="0"/>
+        <f>(F15/J15)-1</f>
         <v>34.616182572614107</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="1"/>
+        <f>(G15/K15)-1</f>
         <v>160.5164986161075</v>
       </c>
       <c r="E15">
@@ -1574,7 +1634,7 @@
         <v>17167</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F15/1000</f>
         <v>1545.03</v>
       </c>
       <c r="H15" s="1">
@@ -1587,7 +1647,7 @@
         <v>482</v>
       </c>
       <c r="K15" s="6">
-        <f t="shared" si="3"/>
+        <f>L15*J15/1000</f>
         <v>9.5657720000000008</v>
       </c>
       <c r="L15" s="5">
@@ -1602,11 +1662,11 @@
         <v>15</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="0"/>
+        <f>(F16/J16)-1</f>
         <v>2.5754716981132075</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="1"/>
+        <f>(G16/K16)-1</f>
         <v>26.534222027054735</v>
       </c>
       <c r="E16">
@@ -1616,7 +1676,7 @@
         <v>379</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F16/1000</f>
         <v>34.11</v>
       </c>
       <c r="H16" s="1">
@@ -1629,7 +1689,7 @@
         <v>106</v>
       </c>
       <c r="K16" s="6">
-        <f t="shared" si="3"/>
+        <f>L16*J16/1000</f>
         <v>1.2388219999999999</v>
       </c>
       <c r="L16" s="5">
@@ -1644,11 +1704,11 @@
         <v>16</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="0"/>
+        <f>(F17/J17)-1</f>
         <v>3.4772727272727275</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="1"/>
+        <f>(G17/K17)-1</f>
         <v>26.926713247941333</v>
       </c>
       <c r="E17">
@@ -1658,7 +1718,7 @@
         <v>197</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="2"/>
+        <f>90*F17/1000</f>
         <v>17.73</v>
       </c>
       <c r="H17" s="1">
@@ -1671,7 +1731,7 @@
         <v>44</v>
       </c>
       <c r="K17" s="6">
-        <f t="shared" si="3"/>
+        <f>L17*J17/1000</f>
         <v>0.634876</v>
       </c>
       <c r="L17" s="5">
@@ -1681,5 +1741,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reorder devices in benchmark table.
</commit_message>
<xml_diff>
--- a/Docs/Attachments/BenchmarksVitis.xlsx
+++ b/Docs/Attachments/BenchmarksVitis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\c-sharp\Hastlayer-SDK-Vitis\Docs\Attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14311D84-2C93-4D69-A776-DDE853578861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E46EB2-995F-4360-A703-77B30994F683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -678,32 +678,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DEFFE78-E3D4-4B7C-9C40-A543930B7FFC}" name="Table1" displayName="Table1" ref="A1:L17" totalsRowShown="0">
-  <autoFilter ref="A1:L17" xr:uid="{8A2D4EA8-9217-4FE5-8D42-089013CF93D2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
-    <sortCondition ref="A1:A17"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3ECD158E-3DBB-4185-8528-A825DEBE360F}" name="Table1" displayName="Table1" ref="A1:L17" totalsRowShown="0">
+  <autoFilter ref="A1:L17" xr:uid="{270411E9-89E0-46FE-9F59-B63F9D56CBA9}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{BCC5BB97-9D21-4C10-A1AC-3169285ACE85}" name="Device"/>
-    <tableColumn id="2" xr3:uid="{E02FF3CC-EF4B-449F-AC35-450BFA13E16F}" name="Algorithm"/>
-    <tableColumn id="3" xr3:uid="{B6499BAC-6A77-45CF-B33A-7834EF7AE07C}" name="Speed advantage" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{E1DA8808-F7B2-4F0F-B73A-67ECA8751623}" name="Device"/>
+    <tableColumn id="2" xr3:uid="{71D8BFBD-053F-486F-9D39-B46ADEC8C2D4}" name="Algorithm"/>
+    <tableColumn id="3" xr3:uid="{E7AA063E-892B-46AA-8C17-E45781DB5404}" name="Speed advantage" dataDxfId="8">
       <calculatedColumnFormula>(F2/J2)-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F534939D-7296-49EA-94FA-117E5B1AD75B}" name="Power advantage" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{1BFB1F6C-B882-42ED-A440-BCF271F2FE6E}" name="Power advantage" dataDxfId="7">
       <calculatedColumnFormula>(G2/K2)-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{9821B29C-FCB1-4C03-A563-1B6291E9CD28}" name="Parallelism"/>
-    <tableColumn id="6" xr3:uid="{D59DCF9C-205F-4833-9388-5263C54DDB8B}" name="CPU" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{1A2039BF-94BA-4B94-903A-588CED48280E}" name="CPU power" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{4CEF6C51-A874-4299-A9DF-AD31F969E138}" name="Parallelism"/>
+    <tableColumn id="6" xr3:uid="{C811A456-DD1E-4667-92ED-CE419599226D}" name="CPU" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{FCE30281-E4B9-4A71-AB54-F1BF19C7F192}" name="CPU power" dataDxfId="5">
       <calculatedColumnFormula>90*F2/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{9D77DFD2-A1F6-455B-A5A6-964B37E62FC4}" name="FPGA utilization" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{0F2C4863-589C-42AC-8BB0-D5F5238E5C6A}" name="Net FPGA" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{17AEC27A-0BAE-4DDB-9FB3-19107E161C70}" name="Total FPGA" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{55E77FEE-ED30-4B73-AE7C-435553A4B7D0}" name="FPGA power" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{67A83361-3ADD-4370-9048-1508C7C469BB}" name="FPGA utilization" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{8DD6EE73-67C9-4026-A08A-CD722EF738AA}" name="Net FPGA" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{4D020E4E-54E2-4695-8B05-74BAA8EA9968}" name="Total FPGA" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{AD6DFD26-235C-4C5F-8EEE-5055721AB74D}" name="FPGA power" dataDxfId="1">
       <calculatedColumnFormula>L2*J2/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{FA68E0D5-D0B6-4FBF-9069-693603D766A2}" name="FPGA on-chip power" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{059C4A3C-3E37-4EDD-A78B-31021367FCC2}" name="FPGA on-chip power" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1009,7 +1006,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,170 +1065,170 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2">
         <f>(F2/J2)-1</f>
-        <v>7.3538461538461544</v>
+        <v>15.90625</v>
       </c>
       <c r="D2" s="2">
         <f>(G2/K2)-1</f>
-        <v>30.472483312242197</v>
+        <v>65.054373779031906</v>
       </c>
       <c r="E2">
         <v>150</v>
       </c>
       <c r="F2" s="3">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="G2" s="4">
         <f>90*F2/1000</f>
-        <v>48.87</v>
+        <v>48.69</v>
       </c>
       <c r="H2" s="1">
-        <v>0.27229999999999999</v>
+        <v>0.21440000000000001</v>
       </c>
       <c r="I2" s="3">
         <v>12</v>
       </c>
       <c r="J2" s="3">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="K2" s="6">
         <f>L2*J2/1000</f>
-        <v>1.5527849999999999</v>
+        <v>0.73712</v>
       </c>
       <c r="L2" s="5">
-        <v>23.888999999999999</v>
+        <v>23.035</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2">
         <f>(F3/J3)-1</f>
-        <v>34.4765485141425</v>
+        <v>34.139676113360323</v>
       </c>
       <c r="D3" s="2">
         <f>(G3/K3)-1</f>
-        <v>132.65521228485181</v>
+        <v>136.29415455621572</v>
       </c>
       <c r="E3">
         <v>150</v>
       </c>
       <c r="F3" s="3">
-        <v>198172</v>
+        <v>17359</v>
       </c>
       <c r="G3" s="4">
         <f>90*F3/1000</f>
-        <v>17835.48</v>
+        <v>1562.31</v>
       </c>
       <c r="H3" s="1">
-        <v>0.27229999999999999</v>
+        <v>0.21440000000000001</v>
       </c>
       <c r="I3" s="3">
-        <v>5340</v>
+        <v>459</v>
       </c>
       <c r="J3" s="3">
-        <v>5586</v>
+        <v>494</v>
       </c>
       <c r="K3" s="6">
         <f>L3*J3/1000</f>
-        <v>133.44395399999999</v>
+        <v>11.379290000000001</v>
       </c>
       <c r="L3" s="5">
-        <v>23.888999999999999</v>
+        <v>23.035</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2">
         <f>(F4/J4)-1</f>
-        <v>1.7071428571428573</v>
+        <v>2.2612612612612613</v>
       </c>
       <c r="D4" s="2">
         <f>(G4/K4)-1</f>
-        <v>14.642196786264583</v>
+        <v>18.583234154891482</v>
       </c>
       <c r="E4">
         <v>300</v>
       </c>
       <c r="F4" s="3">
-        <v>379</v>
+        <v>362</v>
       </c>
       <c r="G4" s="4">
         <f>90*F4/1000</f>
-        <v>34.11</v>
+        <v>32.58</v>
       </c>
       <c r="H4" s="1">
-        <v>0.15559999999999999</v>
+        <v>0.1086</v>
       </c>
       <c r="I4" s="3">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="J4" s="3">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="K4" s="6">
         <f>L4*J4/1000</f>
-        <v>2.1806399999999999</v>
+        <v>1.6636679999999999</v>
       </c>
       <c r="L4" s="5">
-        <v>15.576000000000001</v>
+        <v>14.988</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="2">
         <f>(F5/J5)-1</f>
-        <v>2.0298507462686568</v>
+        <v>3.8684210526315788</v>
       </c>
       <c r="D5" s="2">
         <f>(G5/K5)-1</f>
-        <v>13.325535443350622</v>
+        <v>23.966261808367072</v>
       </c>
       <c r="E5">
         <v>230</v>
       </c>
       <c r="F5" s="3">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="G5" s="4">
         <f>90*F5/1000</f>
-        <v>18.27</v>
+        <v>16.649999999999999</v>
       </c>
       <c r="H5" s="1">
-        <v>0.1857</v>
+        <v>0.1363</v>
       </c>
       <c r="I5" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" s="3">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="K5" s="6">
         <f>L5*J5/1000</f>
-        <v>1.275345</v>
+        <v>0.66689999999999994</v>
       </c>
       <c r="L5" s="5">
-        <v>19.035</v>
+        <v>17.55</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1404,170 +1401,170 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2">
         <f>(F10/J10)-1</f>
-        <v>15.90625</v>
+        <v>7.3538461538461544</v>
       </c>
       <c r="D10" s="2">
         <f>(G10/K10)-1</f>
-        <v>65.054373779031906</v>
+        <v>30.472483312242197</v>
       </c>
       <c r="E10">
         <v>150</v>
       </c>
       <c r="F10" s="3">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="G10" s="4">
         <f>90*F10/1000</f>
-        <v>48.69</v>
+        <v>48.87</v>
       </c>
       <c r="H10" s="1">
-        <v>0.21440000000000001</v>
+        <v>0.27229999999999999</v>
       </c>
       <c r="I10" s="3">
         <v>12</v>
       </c>
       <c r="J10" s="3">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="K10" s="6">
         <f>L10*J10/1000</f>
-        <v>0.73712</v>
+        <v>1.5527849999999999</v>
       </c>
       <c r="L10" s="5">
-        <v>23.035</v>
+        <v>23.888999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2">
         <f>(F11/J11)-1</f>
-        <v>34.139676113360323</v>
+        <v>34.4765485141425</v>
       </c>
       <c r="D11" s="2">
         <f>(G11/K11)-1</f>
-        <v>136.29415455621572</v>
+        <v>132.65521228485181</v>
       </c>
       <c r="E11">
         <v>150</v>
       </c>
       <c r="F11" s="3">
-        <v>17359</v>
+        <v>198172</v>
       </c>
       <c r="G11" s="4">
         <f>90*F11/1000</f>
-        <v>1562.31</v>
+        <v>17835.48</v>
       </c>
       <c r="H11" s="1">
-        <v>0.21440000000000001</v>
+        <v>0.27229999999999999</v>
       </c>
       <c r="I11" s="3">
-        <v>459</v>
+        <v>5340</v>
       </c>
       <c r="J11" s="3">
-        <v>494</v>
+        <v>5586</v>
       </c>
       <c r="K11" s="6">
         <f>L11*J11/1000</f>
-        <v>11.379290000000001</v>
+        <v>133.44395399999999</v>
       </c>
       <c r="L11" s="5">
-        <v>23.035</v>
+        <v>23.888999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="2">
         <f>(F12/J12)-1</f>
-        <v>2.2612612612612613</v>
+        <v>1.7071428571428573</v>
       </c>
       <c r="D12" s="2">
         <f>(G12/K12)-1</f>
-        <v>18.583234154891482</v>
+        <v>14.642196786264583</v>
       </c>
       <c r="E12">
         <v>300</v>
       </c>
       <c r="F12" s="3">
-        <v>362</v>
+        <v>379</v>
       </c>
       <c r="G12" s="4">
         <f>90*F12/1000</f>
-        <v>32.58</v>
+        <v>34.11</v>
       </c>
       <c r="H12" s="1">
-        <v>0.1086</v>
+        <v>0.15559999999999999</v>
       </c>
       <c r="I12" s="3">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="J12" s="3">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="K12" s="6">
         <f>L12*J12/1000</f>
-        <v>1.6636679999999999</v>
+        <v>2.1806399999999999</v>
       </c>
       <c r="L12" s="5">
-        <v>14.988</v>
+        <v>15.576000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="2">
         <f>(F13/J13)-1</f>
-        <v>3.8684210526315788</v>
+        <v>2.0298507462686568</v>
       </c>
       <c r="D13" s="2">
         <f>(G13/K13)-1</f>
-        <v>23.966261808367072</v>
+        <v>13.325535443350622</v>
       </c>
       <c r="E13">
         <v>230</v>
       </c>
       <c r="F13" s="3">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="G13" s="4">
         <f>90*F13/1000</f>
-        <v>16.649999999999999</v>
+        <v>18.27</v>
       </c>
       <c r="H13" s="1">
-        <v>0.1363</v>
+        <v>0.1857</v>
       </c>
       <c r="I13" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J13" s="3">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="K13" s="6">
         <f>L13*J13/1000</f>
-        <v>0.66689999999999994</v>
+        <v>1.275345</v>
       </c>
       <c r="L13" s="5">
-        <v>17.55</v>
+        <v>19.035</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removing <sup>s from the Excel spreadsheet
</commit_message>
<xml_diff>
--- a/Docs/Attachments/BenchmarksVitis.xlsx
+++ b/Docs/Attachments/BenchmarksVitis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\c-sharp\Hastlayer-SDK-Vitis\Docs\Attachments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Hastlayer\Hastlayer-SDK2\Docs\Attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E46EB2-995F-4360-A703-77B30994F683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE88DEA-5E16-4805-9EA4-947D147846F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="240" windowWidth="51600" windowHeight="20760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>Device</t>
   </si>
@@ -72,12 +71,6 @@
     <t>Alveo U200</t>
   </si>
   <si>
-    <t>ImageContrastModifier&lt;sup&gt;1&lt;/sup&gt;</t>
-  </si>
-  <si>
-    <t>ImageContrastModifier&lt;sup&gt;2&lt;/sup&gt;</t>
-  </si>
-  <si>
     <t>ParallelAlgorithm</t>
   </si>
   <si>
@@ -90,10 +83,10 @@
     <t>Alveo U280</t>
   </si>
   <si>
-    <t>ImageContrastModifier&lt;sup&gt;3&lt;/sup&gt;</t>
-  </si>
-  <si>
     <t>Alveo U50</t>
+  </si>
+  <si>
+    <t>ImageContrastModifier</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +999,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,17 +1058,17 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" s="2">
-        <f>(F2/J2)-1</f>
+        <f t="shared" ref="C2:C17" si="0">(F2/J2)-1</f>
         <v>15.90625</v>
       </c>
       <c r="D2" s="2">
-        <f>(G2/K2)-1</f>
+        <f t="shared" ref="D2:D17" si="1">(G2/K2)-1</f>
         <v>65.054373779031906</v>
       </c>
       <c r="E2">
@@ -1085,7 +1078,7 @@
         <v>541</v>
       </c>
       <c r="G2" s="4">
-        <f>90*F2/1000</f>
+        <f t="shared" ref="G2:G17" si="2">90*F2/1000</f>
         <v>48.69</v>
       </c>
       <c r="H2" s="1">
@@ -1098,7 +1091,7 @@
         <v>32</v>
       </c>
       <c r="K2" s="6">
-        <f>L2*J2/1000</f>
+        <f t="shared" ref="K2:K17" si="3">L2*J2/1000</f>
         <v>0.73712</v>
       </c>
       <c r="L2" s="5">
@@ -1107,17 +1100,17 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
       <c r="C3" s="2">
-        <f>(F3/J3)-1</f>
+        <f t="shared" si="0"/>
         <v>34.139676113360323</v>
       </c>
       <c r="D3" s="2">
-        <f>(G3/K3)-1</f>
+        <f t="shared" si="1"/>
         <v>136.29415455621572</v>
       </c>
       <c r="E3">
@@ -1127,7 +1120,7 @@
         <v>17359</v>
       </c>
       <c r="G3" s="4">
-        <f>90*F3/1000</f>
+        <f t="shared" si="2"/>
         <v>1562.31</v>
       </c>
       <c r="H3" s="1">
@@ -1140,7 +1133,7 @@
         <v>494</v>
       </c>
       <c r="K3" s="6">
-        <f>L3*J3/1000</f>
+        <f t="shared" si="3"/>
         <v>11.379290000000001</v>
       </c>
       <c r="L3" s="5">
@@ -1149,17 +1142,17 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2">
-        <f>(F4/J4)-1</f>
+        <f t="shared" si="0"/>
         <v>2.2612612612612613</v>
       </c>
       <c r="D4" s="2">
-        <f>(G4/K4)-1</f>
+        <f t="shared" si="1"/>
         <v>18.583234154891482</v>
       </c>
       <c r="E4">
@@ -1169,7 +1162,7 @@
         <v>362</v>
       </c>
       <c r="G4" s="4">
-        <f>90*F4/1000</f>
+        <f t="shared" si="2"/>
         <v>32.58</v>
       </c>
       <c r="H4" s="1">
@@ -1182,7 +1175,7 @@
         <v>111</v>
       </c>
       <c r="K4" s="6">
-        <f>L4*J4/1000</f>
+        <f t="shared" si="3"/>
         <v>1.6636679999999999</v>
       </c>
       <c r="L4" s="5">
@@ -1191,17 +1184,17 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2">
-        <f>(F5/J5)-1</f>
+        <f t="shared" si="0"/>
         <v>3.8684210526315788</v>
       </c>
       <c r="D5" s="2">
-        <f>(G5/K5)-1</f>
+        <f t="shared" si="1"/>
         <v>23.966261808367072</v>
       </c>
       <c r="E5">
@@ -1211,7 +1204,7 @@
         <v>185</v>
       </c>
       <c r="G5" s="4">
-        <f>90*F5/1000</f>
+        <f t="shared" si="2"/>
         <v>16.649999999999999</v>
       </c>
       <c r="H5" s="1">
@@ -1224,7 +1217,7 @@
         <v>38</v>
       </c>
       <c r="K5" s="6">
-        <f>L5*J5/1000</f>
+        <f t="shared" si="3"/>
         <v>0.66689999999999994</v>
       </c>
       <c r="L5" s="5">
@@ -1233,17 +1226,17 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2">
-        <f>(F6/J6)-1</f>
+        <f t="shared" si="0"/>
         <v>15.030303030303031</v>
       </c>
       <c r="D6" s="2">
-        <f>(G6/K6)-1</f>
+        <f t="shared" si="1"/>
         <v>56.214755422242725</v>
       </c>
       <c r="E6">
@@ -1253,7 +1246,7 @@
         <v>529</v>
       </c>
       <c r="G6" s="4">
-        <f>90*F6/1000</f>
+        <f t="shared" si="2"/>
         <v>47.61</v>
       </c>
       <c r="H6" s="1">
@@ -1266,7 +1259,7 @@
         <v>33</v>
       </c>
       <c r="K6" s="6">
-        <f>L6*J6/1000</f>
+        <f t="shared" si="3"/>
         <v>0.83212800000000009</v>
       </c>
       <c r="L6" s="5">
@@ -1275,17 +1268,17 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2">
-        <f>(F7/J7)-1</f>
+        <f t="shared" si="0"/>
         <v>32.680557977332171</v>
       </c>
       <c r="D7" s="2">
-        <f>(G7/K7)-1</f>
+        <f t="shared" si="1"/>
         <v>119.21138237467859</v>
       </c>
       <c r="E7">
@@ -1295,7 +1288,7 @@
         <v>193158</v>
       </c>
       <c r="G7" s="4">
-        <f>90*F7/1000</f>
+        <f t="shared" si="2"/>
         <v>17384.22</v>
       </c>
       <c r="H7" s="1">
@@ -1308,7 +1301,7 @@
         <v>5735</v>
       </c>
       <c r="K7" s="6">
-        <f>L7*J7/1000</f>
+        <f t="shared" si="3"/>
         <v>144.61376000000001</v>
       </c>
       <c r="L7" s="5">
@@ -1317,17 +1310,17 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2">
-        <f>(F8/J8)-1</f>
+        <f t="shared" si="0"/>
         <v>3.568807339449541</v>
       </c>
       <c r="D8" s="2">
-        <f>(G8/K8)-1</f>
+        <f t="shared" si="1"/>
         <v>24.371300089495815</v>
       </c>
       <c r="E8">
@@ -1337,7 +1330,7 @@
         <v>498</v>
       </c>
       <c r="G8" s="4">
-        <f>90*F8/1000</f>
+        <f t="shared" si="2"/>
         <v>44.82</v>
       </c>
       <c r="H8" s="1">
@@ -1350,7 +1343,7 @@
         <v>109</v>
       </c>
       <c r="K8" s="6">
-        <f>L8*J8/1000</f>
+        <f t="shared" si="3"/>
         <v>1.7665630000000001</v>
       </c>
       <c r="L8" s="5">
@@ -1359,17 +1352,17 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2">
-        <f>(F9/J9)-1</f>
+        <f t="shared" si="0"/>
         <v>3.6904761904761907</v>
       </c>
       <c r="D9" s="2">
-        <f>(G9/K9)-1</f>
+        <f t="shared" si="1"/>
         <v>20.222807156143844</v>
       </c>
       <c r="E9">
@@ -1379,7 +1372,7 @@
         <v>197</v>
       </c>
       <c r="G9" s="4">
-        <f>90*F9/1000</f>
+        <f t="shared" si="2"/>
         <v>17.73</v>
       </c>
       <c r="H9" s="1">
@@ -1392,7 +1385,7 @@
         <v>42</v>
       </c>
       <c r="K9" s="6">
-        <f>L9*J9/1000</f>
+        <f t="shared" si="3"/>
         <v>0.83542199999999989</v>
       </c>
       <c r="L9" s="5">
@@ -1404,14 +1397,14 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2">
-        <f>(F10/J10)-1</f>
+        <f t="shared" si="0"/>
         <v>7.3538461538461544</v>
       </c>
       <c r="D10" s="2">
-        <f>(G10/K10)-1</f>
+        <f t="shared" si="1"/>
         <v>30.472483312242197</v>
       </c>
       <c r="E10">
@@ -1421,7 +1414,7 @@
         <v>543</v>
       </c>
       <c r="G10" s="4">
-        <f>90*F10/1000</f>
+        <f t="shared" si="2"/>
         <v>48.87</v>
       </c>
       <c r="H10" s="1">
@@ -1434,7 +1427,7 @@
         <v>65</v>
       </c>
       <c r="K10" s="6">
-        <f>L10*J10/1000</f>
+        <f t="shared" si="3"/>
         <v>1.5527849999999999</v>
       </c>
       <c r="L10" s="5">
@@ -1446,14 +1439,14 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2">
-        <f>(F11/J11)-1</f>
+        <f t="shared" si="0"/>
         <v>34.4765485141425</v>
       </c>
       <c r="D11" s="2">
-        <f>(G11/K11)-1</f>
+        <f t="shared" si="1"/>
         <v>132.65521228485181</v>
       </c>
       <c r="E11">
@@ -1463,7 +1456,7 @@
         <v>198172</v>
       </c>
       <c r="G11" s="4">
-        <f>90*F11/1000</f>
+        <f t="shared" si="2"/>
         <v>17835.48</v>
       </c>
       <c r="H11" s="1">
@@ -1476,7 +1469,7 @@
         <v>5586</v>
       </c>
       <c r="K11" s="6">
-        <f>L11*J11/1000</f>
+        <f t="shared" si="3"/>
         <v>133.44395399999999</v>
       </c>
       <c r="L11" s="5">
@@ -1488,14 +1481,14 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2">
-        <f>(F12/J12)-1</f>
+        <f t="shared" si="0"/>
         <v>1.7071428571428573</v>
       </c>
       <c r="D12" s="2">
-        <f>(G12/K12)-1</f>
+        <f t="shared" si="1"/>
         <v>14.642196786264583</v>
       </c>
       <c r="E12">
@@ -1505,7 +1498,7 @@
         <v>379</v>
       </c>
       <c r="G12" s="4">
-        <f>90*F12/1000</f>
+        <f t="shared" si="2"/>
         <v>34.11</v>
       </c>
       <c r="H12" s="1">
@@ -1518,7 +1511,7 @@
         <v>140</v>
       </c>
       <c r="K12" s="6">
-        <f>L12*J12/1000</f>
+        <f t="shared" si="3"/>
         <v>2.1806399999999999</v>
       </c>
       <c r="L12" s="5">
@@ -1530,14 +1523,14 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2">
-        <f>(F13/J13)-1</f>
+        <f t="shared" si="0"/>
         <v>2.0298507462686568</v>
       </c>
       <c r="D13" s="2">
-        <f>(G13/K13)-1</f>
+        <f t="shared" si="1"/>
         <v>13.325535443350622</v>
       </c>
       <c r="E13">
@@ -1547,7 +1540,7 @@
         <v>203</v>
       </c>
       <c r="G13" s="4">
-        <f>90*F13/1000</f>
+        <f t="shared" si="2"/>
         <v>18.27</v>
       </c>
       <c r="H13" s="1">
@@ -1560,7 +1553,7 @@
         <v>67</v>
       </c>
       <c r="K13" s="6">
-        <f>L13*J13/1000</f>
+        <f t="shared" si="3"/>
         <v>1.275345</v>
       </c>
       <c r="L13" s="5">
@@ -1569,17 +1562,17 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2">
-        <f>(F14/J14)-1</f>
+        <f t="shared" si="0"/>
         <v>13.242424242424242</v>
       </c>
       <c r="D14" s="2">
-        <f>(G14/K14)-1</f>
+        <f t="shared" si="1"/>
         <v>63.588238527571392</v>
       </c>
       <c r="E14">
@@ -1589,7 +1582,7 @@
         <v>470</v>
       </c>
       <c r="G14" s="4">
-        <f>90*F14/1000</f>
+        <f t="shared" si="2"/>
         <v>42.3</v>
       </c>
       <c r="H14" s="1">
@@ -1602,7 +1595,7 @@
         <v>33</v>
       </c>
       <c r="K14" s="6">
-        <f>L14*J14/1000</f>
+        <f t="shared" si="3"/>
         <v>0.654918</v>
       </c>
       <c r="L14" s="5">
@@ -1611,17 +1604,17 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2">
-        <f>(F15/J15)-1</f>
+        <f t="shared" si="0"/>
         <v>34.616182572614107</v>
       </c>
       <c r="D15" s="2">
-        <f>(G15/K15)-1</f>
+        <f t="shared" si="1"/>
         <v>160.5164986161075</v>
       </c>
       <c r="E15">
@@ -1631,7 +1624,7 @@
         <v>17167</v>
       </c>
       <c r="G15" s="4">
-        <f>90*F15/1000</f>
+        <f t="shared" si="2"/>
         <v>1545.03</v>
       </c>
       <c r="H15" s="1">
@@ -1644,7 +1637,7 @@
         <v>482</v>
       </c>
       <c r="K15" s="6">
-        <f>L15*J15/1000</f>
+        <f t="shared" si="3"/>
         <v>9.5657720000000008</v>
       </c>
       <c r="L15" s="5">
@@ -1653,17 +1646,17 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2">
-        <f>(F16/J16)-1</f>
+        <f t="shared" si="0"/>
         <v>2.5754716981132075</v>
       </c>
       <c r="D16" s="2">
-        <f>(G16/K16)-1</f>
+        <f t="shared" si="1"/>
         <v>26.534222027054735</v>
       </c>
       <c r="E16">
@@ -1673,7 +1666,7 @@
         <v>379</v>
       </c>
       <c r="G16" s="4">
-        <f>90*F16/1000</f>
+        <f t="shared" si="2"/>
         <v>34.11</v>
       </c>
       <c r="H16" s="1">
@@ -1686,7 +1679,7 @@
         <v>106</v>
       </c>
       <c r="K16" s="6">
-        <f>L16*J16/1000</f>
+        <f t="shared" si="3"/>
         <v>1.2388219999999999</v>
       </c>
       <c r="L16" s="5">
@@ -1695,17 +1688,17 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2">
-        <f>(F17/J17)-1</f>
+        <f t="shared" si="0"/>
         <v>3.4772727272727275</v>
       </c>
       <c r="D17" s="2">
-        <f>(G17/K17)-1</f>
+        <f t="shared" si="1"/>
         <v>26.926713247941333</v>
       </c>
       <c r="E17">
@@ -1715,7 +1708,7 @@
         <v>197</v>
       </c>
       <c r="G17" s="4">
-        <f>90*F17/1000</f>
+        <f t="shared" si="2"/>
         <v>17.73</v>
       </c>
       <c r="H17" s="1">
@@ -1728,7 +1721,7 @@
         <v>44</v>
       </c>
       <c r="K17" s="6">
-        <f>L17*J17/1000</f>
+        <f t="shared" si="3"/>
         <v>0.634876</v>
       </c>
       <c r="L17" s="5">

</xml_diff>